<commit_message>
opt@3.1.0#:modify app h5 interface.
</commit_message>
<xml_diff>
--- a/docs/App_Api/Renter_2.0.0/app接口文档规范_v1.1_HTML嵌入.xlsx
+++ b/docs/App_Api/Renter_2.0.0/app接口文档规范_v1.1_HTML嵌入.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>用户使用条款和隐私声明</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -238,10 +238,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>{"head":{"userId":"","token":"","os":"","osVersion":"","appVersion":"","model":"","uuid":"","channel":"租客app","key":""}}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>{"head":{"userId":"","token":"","os":"","osVersion":"","appVersion":"","model":"","uuid":"","channel":"租客app","key":""},"para":{"id":"房间ID"}}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -250,7 +246,30 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>备注：H5页面访问方式由原来的GET改为POST</t>
+    <t>出参</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>html文本</t>
+  </si>
+  <si>
+    <t>html文本</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注：某些H5页面访问方式由原来的GET改为POST</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -258,7 +277,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,8 +334,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="幼圆"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +358,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -419,7 +451,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -428,8 +460,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
@@ -451,6 +486,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -465,8 +503,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="差" xfId="4" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="3" builtinId="8"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
@@ -761,11 +802,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -775,35 +816,37 @@
     <col min="3" max="3" width="12.125" customWidth="1"/>
     <col min="4" max="4" width="20.125" customWidth="1"/>
     <col min="5" max="5" width="34.75" customWidth="1"/>
-    <col min="6" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="29.125" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-    <col min="10" max="10" width="30.25" customWidth="1"/>
+    <col min="6" max="6" width="14.25" customWidth="1"/>
+    <col min="7" max="8" width="15.375" customWidth="1"/>
+    <col min="9" max="9" width="29.125" customWidth="1"/>
+    <col min="10" max="10" width="28" customWidth="1"/>
+    <col min="11" max="11" width="30.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="17"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="17" t="s">
+        <v>62</v>
+      </c>
       <c r="H1" s="18"/>
-      <c r="I1" s="9"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -820,16 +863,19 @@
         <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,25 +883,28 @@
         <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -872,16 +921,19 @@
         <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -898,16 +950,19 @@
         <v>49</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
@@ -924,16 +979,19 @@
         <v>52</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -944,22 +1002,25 @@
         <v>48</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
@@ -976,16 +1037,19 @@
         <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -1002,16 +1066,19 @@
         <v>52</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
@@ -1019,25 +1086,28 @@
         <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
@@ -1054,19 +1124,22 @@
         <v>53</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
opt@3.0.3#:add security h5 for book.
</commit_message>
<xml_diff>
--- a/docs/App_Api/Renter_2.0.0/app接口文档规范_v1.1_HTML嵌入.xlsx
+++ b/docs/App_Api/Renter_2.0.0/app接口文档规范_v1.1_HTML嵌入.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
   <si>
     <t>用户使用条款和隐私声明</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -270,6 +270,21 @@
   </si>
   <si>
     <t>无</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/pages/terms/book.jsp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>预订协议</t>
+  </si>
+  <si>
+    <t>http://{domain}/securityH5/book</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -801,11 +816,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -911,7 +926,7 @@
         <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>60</v>
@@ -1133,6 +1148,35 @@
       </c>
       <c r="I11" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1152,8 +1196,9 @@
     <hyperlink ref="B8" r:id="rId8" display="http://www.mogoroom.com/h5/installment"/>
     <hyperlink ref="B9" r:id="rId9" display="http://www.mogoroom.com/h5/safeguard"/>
     <hyperlink ref="B11" r:id="rId10" display="http://api.mogoroom.com/h5/budget"/>
+    <hyperlink ref="B12" r:id="rId11" display="http://api.mogoroom.com/h5/budget"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>